<commit_message>
new field added - feedback text
</commit_message>
<xml_diff>
--- a/preprocessing_scripts/SurveyResponsesInExcelPythonCode.xlsx
+++ b/preprocessing_scripts/SurveyResponsesInExcelPythonCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varshahindupur/Downloads/RA_Online_Instrument/preprocessing_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33518BFE-7931-1C4F-883A-4BF59358CFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AD95EF-1CC0-7944-8CF6-5878F11CF3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="274">
   <si>
     <t>prolific_id</t>
   </si>
@@ -568,7 +568,22 @@
     <t>https://app.prolific.com/submissions/complete?cc=C18WFMT1</t>
   </si>
   <si>
-    <t>thisisadummytrialprolifi</t>
+    <t>66c8ebb8c2c8d2b4d0424245</t>
+  </si>
+  <si>
+    <t>5d654282986878001c2a5db7</t>
+  </si>
+  <si>
+    <t>exactly-$102</t>
+  </si>
+  <si>
+    <t>more-than-today</t>
+  </si>
+  <si>
+    <t>672f46958f6daac3c8e3bb7a</t>
+  </si>
+  <si>
+    <t>671bb583832abc2b597f794d</t>
   </si>
   <si>
     <t>exactly-today</t>
@@ -577,28 +592,267 @@
     <t>do-not-know</t>
   </si>
   <si>
-    <t>same,different,same,different,same,different,same,different</t>
-  </si>
-  <si>
-    <t>different,same,different,same,different,same,different,same</t>
-  </si>
-  <si>
-    <t>ghggggghhjjkklkll;;,liuuygyftfrtderserses45fyfvgcfffgfggg</t>
+    <t>less-than-$102</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>different,same,different,different,different,same,different,same</t>
+  </si>
+  <si>
+    <t>same,same,different,same,different,same,same,same</t>
+  </si>
+  <si>
+    <t>different,same,different,same,same,same,different,same</t>
+  </si>
+  <si>
+    <t>different,different,different,different,same,same,same,different</t>
+  </si>
+  <si>
+    <t>same,same,different,different,same,same,different,different</t>
+  </si>
+  <si>
+    <t>same,same,different,same,same,different,different,same</t>
+  </si>
+  <si>
+    <t>same,,,,,,,</t>
+  </si>
+  <si>
+    <t>same,same,,,,,,</t>
+  </si>
+  <si>
+    <t>25 cents</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>,,,,different,same,different,same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to build houses and buildings
+to build a firepit
+weights
+to build walkways and sidewalks/streets??
+</t>
+  </si>
+  <si>
+    <t>same,same,same,different,same,same,different,same</t>
+  </si>
+  <si>
+    <t>same,same,different,same,same,same,same,different</t>
+  </si>
+  <si>
+    <t>same,different,same,same,same,same,different,</t>
+  </si>
+  <si>
+    <t>different,same,different,same,same,different,same,different</t>
+  </si>
+  <si>
+    <t xml:space="preserve">construction of walls
+construction of pavement
+chimney and fireplaces
+</t>
+  </si>
+  <si>
+    <t>66ce77e3d21bb5b5d6a83d37</t>
+  </si>
+  <si>
+    <t>same,same,different,different,different,same,different,different</t>
+  </si>
+  <si>
+    <t>same,different,same,same,different,different,same,same</t>
+  </si>
+  <si>
+    <t>same,same,same,different,different,different,different,same</t>
+  </si>
+  <si>
+    <t>same,same,different,different,different,different,different,</t>
+  </si>
+  <si>
+    <t>US and Mexico</t>
+  </si>
+  <si>
+    <t>[70.16, 124.84, 44.78, 26.59, 25.66, 13.31, 14.25, 16.27, 14.54, 16.19, 11.52, 34.59, 6.4, 31.25, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[[74.27, 81.22, 6.84, 48.12]]</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Some college</t>
+  </si>
+  <si>
+    <t>Less than one</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>foundation laying
+construction of ghetters
+drainage system
+building of house</t>
+  </si>
+  <si>
+    <t>Structural-Bar-Dashboard</t>
+  </si>
+  <si>
+    <t>[175.75, 85.93, 76.06, 63.89, 62.42, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[[0, 128.81, 0, 0]]</t>
+  </si>
+  <si>
+    <t>/structure-bar-dashboard</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
   <si>
     <t>TimeSeries-Bar-Dashboard</t>
   </si>
   <si>
-    <t>[7.33, 6.62, 7.67, 0.82, 1.5, 0.99, 0.46, 0.31, 0.31, 0.7, 1.87, 5.18, 2.26, 2.1, 1.08, 1.73, 1.5, 1.91, 1.13, 1.87, 0.45, 0.42, 1.72, 2.04]</t>
-  </si>
-  <si>
-    <t>[[2.02, 4.11, 0, 1.92]]</t>
-  </si>
-  <si>
-    <t>failed</t>
+    <t>[55.38, 51.28, 103.03, 62.72, 15.12, 141.34, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>[[0, 0, 0, 0]]</t>
   </si>
   <si>
     <t>/timeseries-bar-dashboard</t>
+  </si>
+  <si>
+    <t>different,different,different,different,same,different,same,different</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>Agriculture, Food and Natural Resources</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Undergraduate degree</t>
+  </si>
+  <si>
+    <t>3-5</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>different,different,,different,same,same,different,same</t>
+  </si>
+  <si>
+    <t>different,same,same,same,different,same,same,different</t>
+  </si>
+  <si>
+    <t>different,same,same,different,same,same,different,same</t>
+  </si>
+  <si>
+    <t>same,same,different,,same,same,different,different</t>
+  </si>
+  <si>
+    <t>different,different,same,same,same,same,same,</t>
+  </si>
+  <si>
+    <t>same,different,same,same,different,same,different,different</t>
+  </si>
+  <si>
+    <t>same,same,different,different,different,different,same,same</t>
+  </si>
+  <si>
+    <t>same,same,same,same,same,same,same,same</t>
+  </si>
+  <si>
+    <t>buile a wall.    build a fence.  build a porch.  Build a well.  make a barrier.  throw it.
+use it like a hammer.   Break a window.  paper weight.  lifting weight.</t>
+  </si>
+  <si>
+    <t>TimeSeries-Col-Dashboard</t>
+  </si>
+  <si>
+    <t>[30.15, 32.17, 39.1, 24.33, 34.97, 22.35, 21.4, 23.67, 32.04, 12.49, 20.49, 14.05, 15.24, 26.98, 24.99, 15.83, 16.05, 18.71, 10.69, 4.05, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>/timeseries-col-dashboard</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>College diploma</t>
+  </si>
+  <si>
+    <t>Architecture and Construction</t>
   </si>
 </sst>
 </file>
@@ -617,21 +871,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -661,12 +908,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,22 +1215,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CT30"/>
+  <dimension ref="A1:CT86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ4" workbookViewId="0">
-      <selection activeCell="CV20" sqref="CV20"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" customWidth="1"/>
-    <col min="77" max="77" width="116.6640625" customWidth="1"/>
-    <col min="78" max="78" width="34.1640625" customWidth="1"/>
-    <col min="92" max="92" width="16" customWidth="1"/>
-    <col min="93" max="93" width="22.6640625" customWidth="1"/>
-    <col min="94" max="94" width="38.5" customWidth="1"/>
-    <col min="95" max="95" width="21.33203125" customWidth="1"/>
-    <col min="96" max="96" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:98" x14ac:dyDescent="0.2">
@@ -1330,7 +1572,7 @@
         <v>0.3</v>
       </c>
       <c r="CN2">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO2" t="s">
         <v>105</v>
@@ -1371,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="CN3">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO3" t="s">
         <v>110</v>
@@ -1421,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="CN4">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO4" t="s">
         <v>111</v>
@@ -1462,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="CN5">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO5" t="s">
         <v>116</v>
@@ -1527,7 +1769,7 @@
         <v>0.4</v>
       </c>
       <c r="CN6">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO6" t="s">
         <v>105</v>
@@ -1598,7 +1840,7 @@
         <v>0.35</v>
       </c>
       <c r="CN7">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO7" t="s">
         <v>106</v>
@@ -1645,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="CN8">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO8" t="s">
         <v>119</v>
@@ -1692,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="CN9">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO9" t="s">
         <v>123</v>
@@ -1757,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="CN10">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO10" t="s">
         <v>127</v>
@@ -1825,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="CN11">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO11" t="s">
         <v>137</v>
@@ -1869,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="CN12">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO12" t="s">
         <v>148</v>
@@ -1910,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="CN13">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO13" t="s">
         <v>151</v>
@@ -1951,7 +2193,7 @@
         <v>0</v>
       </c>
       <c r="CN14">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO14" t="s">
         <v>153</v>
@@ -2058,7 +2300,7 @@
         <v>0.85</v>
       </c>
       <c r="CN15">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO15" t="s">
         <v>165</v>
@@ -2114,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="CN16">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO16" t="s">
         <v>166</v>
@@ -2132,53 +2374,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>18</v>
       </c>
-      <c r="BY17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BZ17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="CH17" s="2" t="s">
+      <c r="BY17" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ17" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH17" t="s">
         <v>176</v>
       </c>
-      <c r="CI17" s="2" t="s">
+      <c r="CI17" t="s">
         <v>177</v>
       </c>
-      <c r="CJ17" s="2" t="s">
+      <c r="CJ17" t="s">
         <v>178</v>
       </c>
-      <c r="CK17" s="2" t="s">
+      <c r="CK17" t="s">
         <v>179</v>
       </c>
-      <c r="CL17" s="2" t="s">
+      <c r="CL17" t="s">
         <v>180</v>
       </c>
-      <c r="CM17" s="2">
-        <v>0</v>
-      </c>
-      <c r="CN17" s="2">
-        <v>6.1</v>
-      </c>
-      <c r="CP17" s="2" t="s">
+      <c r="CM17">
+        <v>0</v>
+      </c>
+      <c r="CN17">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CP17" t="s">
         <v>181</v>
       </c>
-      <c r="CQ17" s="2" t="s">
+      <c r="CQ17" t="s">
         <v>166</v>
       </c>
-      <c r="CS17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="CT17" s="2">
+      <c r="CS17" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT17">
         <v>0</v>
       </c>
     </row>
@@ -2202,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="CN18">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO18" t="s">
         <v>110</v>
@@ -2225,22 +2467,13 @@
     </row>
     <row r="19" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F19" t="s">
-        <v>184</v>
+        <v>1</v>
       </c>
       <c r="BY19" t="s">
         <v>104</v>
@@ -2252,13 +2485,13 @@
         <v>0</v>
       </c>
       <c r="CN19">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO19" t="s">
+        <v>110</v>
+      </c>
+      <c r="CP19" t="s">
         <v>111</v>
-      </c>
-      <c r="CP19" t="s">
-        <v>116</v>
       </c>
       <c r="CQ19" t="s">
         <v>110</v>
@@ -2275,13 +2508,22 @@
     </row>
     <row r="20" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" t="s">
+        <v>115</v>
       </c>
       <c r="BY20" t="s">
         <v>104</v>
@@ -2293,16 +2535,16 @@
         <v>0</v>
       </c>
       <c r="CN20">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO20" t="s">
+        <v>111</v>
+      </c>
+      <c r="CP20" t="s">
         <v>116</v>
       </c>
-      <c r="CP20" t="s">
-        <v>105</v>
-      </c>
       <c r="CQ20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="CR20">
         <v>0</v>
@@ -2316,16 +2558,13 @@
     </row>
     <row r="21" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="G21" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="BY21" t="s">
         <v>104</v>
@@ -2337,16 +2576,16 @@
         <v>0</v>
       </c>
       <c r="CN21">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO21" t="s">
+        <v>116</v>
+      </c>
+      <c r="CP21" t="s">
         <v>105</v>
       </c>
-      <c r="CP21" t="s">
-        <v>106</v>
-      </c>
       <c r="CQ21" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="CR21">
         <v>0</v>
@@ -2360,13 +2599,13 @@
     </row>
     <row r="22" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BY22" t="s">
         <v>104</v>
@@ -2378,16 +2617,16 @@
         <v>0</v>
       </c>
       <c r="CN22">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO22" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="CP22" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="CQ22" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="CR22">
         <v>0</v>
@@ -2401,19 +2640,13 @@
     </row>
     <row r="23" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>186</v>
+        <v>1</v>
       </c>
       <c r="BY23" t="s">
         <v>104</v>
@@ -2425,16 +2658,16 @@
         <v>0</v>
       </c>
       <c r="CN23">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO23" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="CP23" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CQ23" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="CR23">
         <v>0</v>
@@ -2451,16 +2684,19 @@
         <v>182</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C24">
-        <v>19</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>126</v>
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" t="s">
+        <v>189</v>
       </c>
       <c r="BY24" t="s">
         <v>104</v>
@@ -2472,16 +2708,16 @@
         <v>0</v>
       </c>
       <c r="CN24">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO24" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CP24" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="CQ24" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="CR24">
         <v>0</v>
@@ -2495,13 +2731,43 @@
     </row>
     <row r="25" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" t="s">
+        <v>103</v>
+      </c>
+      <c r="L25" t="s">
+        <v>101</v>
+      </c>
+      <c r="M25" t="s">
+        <v>101</v>
+      </c>
+      <c r="N25" t="s">
+        <v>101</v>
+      </c>
+      <c r="O25" t="s">
+        <v>100</v>
+      </c>
+      <c r="P25" t="s">
+        <v>99</v>
       </c>
       <c r="BY25" t="s">
         <v>104</v>
@@ -2510,19 +2776,19 @@
         <v>104</v>
       </c>
       <c r="CM25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="CN25">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO25" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="CP25" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="CQ25" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="CR25">
         <v>0</v>
@@ -2539,10 +2805,10 @@
         <v>182</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="BY26" t="s">
         <v>104</v>
@@ -2554,16 +2820,16 @@
         <v>0</v>
       </c>
       <c r="CN26">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO26" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="CP26" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="CQ26" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="CR26">
         <v>0</v>
@@ -2577,16 +2843,22 @@
     </row>
     <row r="27" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="C27">
-        <v>11</v>
-      </c>
-      <c r="AZ27" t="s">
-        <v>187</v>
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" t="s">
+        <v>115</v>
       </c>
       <c r="BY27" t="s">
         <v>104</v>
@@ -2598,16 +2870,16 @@
         <v>0</v>
       </c>
       <c r="CN27">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO27" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="CP27" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="CQ27" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="CR27">
         <v>0</v>
@@ -2621,13 +2893,22 @@
     </row>
     <row r="28" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="C28">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" t="s">
+        <v>191</v>
       </c>
       <c r="BY28" t="s">
         <v>104</v>
@@ -2639,16 +2920,16 @@
         <v>0</v>
       </c>
       <c r="CN28">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO28" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="CP28" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="CQ28" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="CR28">
         <v>0</v>
@@ -2662,13 +2943,43 @@
     </row>
     <row r="29" spans="1:98" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="C29">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>101</v>
+      </c>
+      <c r="R29" t="s">
+        <v>103</v>
+      </c>
+      <c r="S29" t="s">
+        <v>99</v>
+      </c>
+      <c r="T29" t="s">
+        <v>102</v>
+      </c>
+      <c r="U29" t="s">
+        <v>102</v>
+      </c>
+      <c r="V29" t="s">
+        <v>103</v>
+      </c>
+      <c r="W29" t="s">
+        <v>100</v>
+      </c>
+      <c r="X29" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>99</v>
       </c>
       <c r="BY29" t="s">
         <v>104</v>
@@ -2677,19 +2988,22 @@
         <v>104</v>
       </c>
       <c r="CM29">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="CN29">
-        <v>6.1</v>
+        <v>9.0499999999999989</v>
       </c>
       <c r="CO29" t="s">
-        <v>153</v>
+        <v>106</v>
+      </c>
+      <c r="CP29" t="s">
+        <v>119</v>
       </c>
       <c r="CQ29" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="CR29">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="CS29" t="b">
         <v>1</v>
@@ -2703,39 +3017,2956 @@
         <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" t="s">
+        <v>101</v>
+      </c>
+      <c r="J30" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY30" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ30" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM30">
+        <v>0.15</v>
+      </c>
+      <c r="CN30">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO30" t="s">
+        <v>105</v>
+      </c>
+      <c r="CP30" t="s">
+        <v>106</v>
+      </c>
+      <c r="CQ30" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR30">
+        <v>0</v>
+      </c>
+      <c r="CS30" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="BY31" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ31" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM31">
+        <v>0</v>
+      </c>
+      <c r="CN31">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO31" t="s">
+        <v>116</v>
+      </c>
+      <c r="CP31" t="s">
+        <v>105</v>
+      </c>
+      <c r="CQ31" t="s">
+        <v>111</v>
+      </c>
+      <c r="CR31">
+        <v>0</v>
+      </c>
+      <c r="CS31" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY32" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ32" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM32">
+        <v>0</v>
+      </c>
+      <c r="CN32">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO32" t="s">
+        <v>119</v>
+      </c>
+      <c r="CP32" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ32" t="s">
+        <v>106</v>
+      </c>
+      <c r="CR32">
+        <v>0</v>
+      </c>
+      <c r="CS32" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>126</v>
+      </c>
+      <c r="BY33" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ33" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM33">
+        <v>0</v>
+      </c>
+      <c r="CN33">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO33" t="s">
+        <v>123</v>
+      </c>
+      <c r="CP33" t="s">
+        <v>127</v>
+      </c>
+      <c r="CQ33" t="s">
+        <v>119</v>
+      </c>
+      <c r="CR33">
+        <v>0</v>
+      </c>
+      <c r="CS33" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>101</v>
+      </c>
+      <c r="R34" t="s">
+        <v>102</v>
+      </c>
+      <c r="S34" t="s">
+        <v>99</v>
+      </c>
+      <c r="T34" t="s">
+        <v>102</v>
+      </c>
+      <c r="U34" t="s">
+        <v>103</v>
+      </c>
+      <c r="V34" t="s">
+        <v>99</v>
+      </c>
+      <c r="W34" t="s">
+        <v>103</v>
+      </c>
+      <c r="X34" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>103</v>
+      </c>
+      <c r="BY34" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ34" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM34">
+        <v>0.3</v>
+      </c>
+      <c r="CN34">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO34" t="s">
+        <v>106</v>
+      </c>
+      <c r="CP34" t="s">
+        <v>119</v>
+      </c>
+      <c r="CQ34" t="s">
+        <v>105</v>
+      </c>
+      <c r="CR34">
+        <v>0</v>
+      </c>
+      <c r="CS34" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="G35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" t="s">
+        <v>102</v>
+      </c>
+      <c r="L35" t="s">
+        <v>100</v>
+      </c>
+      <c r="M35" t="s">
+        <v>101</v>
+      </c>
+      <c r="N35" t="s">
+        <v>100</v>
+      </c>
+      <c r="O35" t="s">
+        <v>102</v>
+      </c>
+      <c r="P35" t="s">
+        <v>101</v>
+      </c>
+      <c r="BY35" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ35" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM35">
+        <v>0.1</v>
+      </c>
+      <c r="CN35">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO35" t="s">
+        <v>105</v>
+      </c>
+      <c r="CP35" t="s">
+        <v>106</v>
+      </c>
+      <c r="CQ35" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR35">
+        <v>0</v>
+      </c>
+      <c r="CS35" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="BY36" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ36" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM36">
+        <v>0</v>
+      </c>
+      <c r="CN36">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO36" t="s">
+        <v>116</v>
+      </c>
+      <c r="CP36" t="s">
+        <v>105</v>
+      </c>
+      <c r="CQ36" t="s">
+        <v>111</v>
+      </c>
+      <c r="CR36">
+        <v>0</v>
+      </c>
+      <c r="CS36" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37">
+        <v>9</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>195</v>
+      </c>
+      <c r="BY37" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ37" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM37">
+        <v>0</v>
+      </c>
+      <c r="CN37">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO37" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP37" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ37" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR37">
+        <v>0</v>
+      </c>
+      <c r="CS37" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>101</v>
+      </c>
+      <c r="R38" t="s">
+        <v>99</v>
+      </c>
+      <c r="S38" t="s">
+        <v>99</v>
+      </c>
+      <c r="T38" t="s">
+        <v>101</v>
+      </c>
+      <c r="U38" t="s">
+        <v>99</v>
+      </c>
+      <c r="V38" t="s">
+        <v>100</v>
+      </c>
+      <c r="W38" t="s">
+        <v>100</v>
+      </c>
+      <c r="X38" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>101</v>
+      </c>
+      <c r="BY38" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ38" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM38">
+        <v>0.15</v>
+      </c>
+      <c r="CN38">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO38" t="s">
+        <v>106</v>
+      </c>
+      <c r="CP38" t="s">
+        <v>119</v>
+      </c>
+      <c r="CQ38" t="s">
+        <v>105</v>
+      </c>
+      <c r="CR38">
+        <v>0</v>
+      </c>
+      <c r="CS38" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY39" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ39" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM39">
+        <v>0</v>
+      </c>
+      <c r="CN39">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO39" t="s">
+        <v>119</v>
+      </c>
+      <c r="CP39" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ39" t="s">
+        <v>106</v>
+      </c>
+      <c r="CR39">
+        <v>0</v>
+      </c>
+      <c r="CS39" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>126</v>
+      </c>
+      <c r="BY40" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ40" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM40">
+        <v>0</v>
+      </c>
+      <c r="CN40">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO40" t="s">
+        <v>123</v>
+      </c>
+      <c r="CP40" t="s">
+        <v>127</v>
+      </c>
+      <c r="CQ40" t="s">
+        <v>119</v>
+      </c>
+      <c r="CR40">
+        <v>0</v>
+      </c>
+      <c r="CS40" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="G41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" t="s">
+        <v>99</v>
+      </c>
+      <c r="I41" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" t="s">
+        <v>100</v>
+      </c>
+      <c r="K41" t="s">
+        <v>101</v>
+      </c>
+      <c r="L41" t="s">
+        <v>101</v>
+      </c>
+      <c r="M41" t="s">
+        <v>102</v>
+      </c>
+      <c r="N41" t="s">
+        <v>101</v>
+      </c>
+      <c r="O41" t="s">
+        <v>103</v>
+      </c>
+      <c r="P41" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY41" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ41" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM41">
+        <v>0.2</v>
+      </c>
+      <c r="CN41">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO41" t="s">
+        <v>105</v>
+      </c>
+      <c r="CP41" t="s">
+        <v>106</v>
+      </c>
+      <c r="CQ41" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR41">
+        <v>0</v>
+      </c>
+      <c r="CS41" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>183</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="AP42" t="s">
+        <v>196</v>
+      </c>
+      <c r="AQ42" t="s">
+        <v>140</v>
+      </c>
+      <c r="AR42" t="s">
+        <v>141</v>
+      </c>
+      <c r="AS42" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT42" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU42" t="s">
+        <v>144</v>
+      </c>
+      <c r="AV42" t="s">
+        <v>197</v>
+      </c>
+      <c r="AW42" t="s">
+        <v>198</v>
+      </c>
+      <c r="BY42" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ42" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM42">
+        <v>0.05</v>
+      </c>
+      <c r="CN42">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO42" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP42" t="s">
+        <v>148</v>
+      </c>
+      <c r="CQ42" t="s">
+        <v>127</v>
+      </c>
+      <c r="CR42">
+        <v>0</v>
+      </c>
+      <c r="CS42" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>199</v>
+      </c>
+      <c r="BY43" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ43" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM43">
+        <v>0</v>
+      </c>
+      <c r="CN43">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO43" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP43" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ43" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR43">
+        <v>0</v>
+      </c>
+      <c r="CS43" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>187</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>101</v>
+      </c>
+      <c r="R44" t="s">
+        <v>103</v>
+      </c>
+      <c r="S44" t="s">
+        <v>99</v>
+      </c>
+      <c r="T44" t="s">
+        <v>103</v>
+      </c>
+      <c r="U44" t="s">
+        <v>103</v>
+      </c>
+      <c r="V44" t="s">
+        <v>102</v>
+      </c>
+      <c r="W44" t="s">
+        <v>101</v>
+      </c>
+      <c r="X44" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>103</v>
+      </c>
+      <c r="BY44" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ44" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM44">
+        <v>0.25</v>
+      </c>
+      <c r="CN44">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO44" t="s">
+        <v>106</v>
+      </c>
+      <c r="CP44" t="s">
+        <v>119</v>
+      </c>
+      <c r="CQ44" t="s">
+        <v>105</v>
+      </c>
+      <c r="CR44">
+        <v>0</v>
+      </c>
+      <c r="CS44" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>186</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>194</v>
+      </c>
+      <c r="BY45" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ45" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM45">
+        <v>0</v>
+      </c>
+      <c r="CN45">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO45" t="s">
+        <v>119</v>
+      </c>
+      <c r="CP45" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ45" t="s">
+        <v>106</v>
+      </c>
+      <c r="CR45">
+        <v>0</v>
+      </c>
+      <c r="CS45" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46">
+        <v>19</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>201</v>
+      </c>
+      <c r="BY46" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ46" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM46">
+        <v>0</v>
+      </c>
+      <c r="CN46">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO46" t="s">
+        <v>123</v>
+      </c>
+      <c r="CP46" t="s">
+        <v>127</v>
+      </c>
+      <c r="CQ46" t="s">
+        <v>119</v>
+      </c>
+      <c r="CR46">
+        <v>0</v>
+      </c>
+      <c r="CS46" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="AP47" t="s">
+        <v>196</v>
+      </c>
+      <c r="AR47" t="s">
+        <v>141</v>
+      </c>
+      <c r="AS47" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT47" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AV47" t="s">
+        <v>202</v>
+      </c>
+      <c r="BY47" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ47" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM47">
+        <v>0.05</v>
+      </c>
+      <c r="CN47">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO47" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP47" t="s">
+        <v>148</v>
+      </c>
+      <c r="CQ47" t="s">
+        <v>127</v>
+      </c>
+      <c r="CR47">
+        <v>0</v>
+      </c>
+      <c r="CS47" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY48" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ48" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM48">
+        <v>0</v>
+      </c>
+      <c r="CN48">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO48" t="s">
+        <v>119</v>
+      </c>
+      <c r="CP48" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ48" t="s">
+        <v>106</v>
+      </c>
+      <c r="CR48">
+        <v>0</v>
+      </c>
+      <c r="CS48" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49">
+        <v>9</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>130</v>
+      </c>
+      <c r="BY49" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ49" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM49">
+        <v>0</v>
+      </c>
+      <c r="CN49">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO49" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP49" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ49" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR49">
+        <v>0</v>
+      </c>
+      <c r="CS49" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50">
+        <v>19</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>126</v>
+      </c>
+      <c r="BY50" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ50" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM50">
+        <v>0</v>
+      </c>
+      <c r="CN50">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO50" t="s">
+        <v>123</v>
+      </c>
+      <c r="CP50" t="s">
+        <v>127</v>
+      </c>
+      <c r="CQ50" t="s">
+        <v>119</v>
+      </c>
+      <c r="CR50">
+        <v>0</v>
+      </c>
+      <c r="CS50" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51">
+        <v>11</v>
+      </c>
+      <c r="AZ51" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY51" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ51" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM51">
+        <v>0</v>
+      </c>
+      <c r="CN51">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO51" t="s">
+        <v>148</v>
+      </c>
+      <c r="CP51" t="s">
+        <v>151</v>
+      </c>
+      <c r="CQ51" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR51">
+        <v>0</v>
+      </c>
+      <c r="CS51" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
+      <c r="BY52" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ52" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM52">
+        <v>0</v>
+      </c>
+      <c r="CN52">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO52" t="s">
+        <v>151</v>
+      </c>
+      <c r="CP52" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ52" t="s">
+        <v>148</v>
+      </c>
+      <c r="CR52">
+        <v>0</v>
+      </c>
+      <c r="CS52" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53">
+        <v>19</v>
+      </c>
+      <c r="BY53" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ53" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM53">
+        <v>0</v>
+      </c>
+      <c r="CN53">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO53" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ53" t="s">
+        <v>151</v>
+      </c>
+      <c r="CR53">
+        <v>1</v>
+      </c>
+      <c r="CS53" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="AP54" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ54" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR54" t="s">
+        <v>206</v>
+      </c>
+      <c r="BY54" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ54" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM54">
+        <v>0</v>
+      </c>
+      <c r="CN54">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO54" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP54" t="s">
+        <v>148</v>
+      </c>
+      <c r="CQ54" t="s">
+        <v>127</v>
+      </c>
+      <c r="CR54">
+        <v>0</v>
+      </c>
+      <c r="CS54" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>187</v>
+      </c>
+      <c r="B55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55">
+        <v>9</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AH55" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ55" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK55" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>135</v>
+      </c>
+      <c r="BY55" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ55" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM55">
+        <v>0.05</v>
+      </c>
+      <c r="CN55">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO55" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP55" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ55" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR55">
+        <v>0</v>
+      </c>
+      <c r="CS55" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56">
+        <v>11</v>
+      </c>
+      <c r="AZ56" t="s">
+        <v>208</v>
+      </c>
+      <c r="BY56" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ56" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM56">
+        <v>0</v>
+      </c>
+      <c r="CN56">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO56" t="s">
+        <v>148</v>
+      </c>
+      <c r="CP56" t="s">
+        <v>151</v>
+      </c>
+      <c r="CQ56" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR56">
+        <v>0</v>
+      </c>
+      <c r="CS56" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="BY57" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ57" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM57">
+        <v>0</v>
+      </c>
+      <c r="CN57">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO57" t="s">
+        <v>151</v>
+      </c>
+      <c r="CP57" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ57" t="s">
+        <v>148</v>
+      </c>
+      <c r="CR57">
+        <v>0</v>
+      </c>
+      <c r="CS57" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58">
+        <v>19</v>
+      </c>
+      <c r="BY58" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ58" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM58">
+        <v>0</v>
+      </c>
+      <c r="CN58">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO58" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ58" t="s">
+        <v>151</v>
+      </c>
+      <c r="CR58">
+        <v>2</v>
+      </c>
+      <c r="CS58" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>209</v>
+      </c>
+      <c r="B59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="BY59" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ59" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM59">
+        <v>0</v>
+      </c>
+      <c r="CN59">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO59" t="s">
+        <v>110</v>
+      </c>
+      <c r="CP59" t="s">
+        <v>111</v>
+      </c>
+      <c r="CQ59" t="s">
+        <v>110</v>
+      </c>
+      <c r="CR59">
+        <v>0</v>
+      </c>
+      <c r="CS59" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="AP60" t="s">
+        <v>210</v>
+      </c>
+      <c r="AQ60" t="s">
+        <v>140</v>
+      </c>
+      <c r="AR60" t="s">
+        <v>141</v>
+      </c>
+      <c r="AS60" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT60" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU60" t="s">
+        <v>144</v>
+      </c>
+      <c r="AV60" t="s">
+        <v>213</v>
+      </c>
+      <c r="BY60" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ60" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM60">
+        <v>0</v>
+      </c>
+      <c r="CN60">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO60" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP60" t="s">
+        <v>148</v>
+      </c>
+      <c r="CQ60" t="s">
+        <v>127</v>
+      </c>
+      <c r="CR60">
+        <v>0</v>
+      </c>
+      <c r="CS60" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>209</v>
+      </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E61" t="s">
+        <v>114</v>
+      </c>
+      <c r="F61" t="s">
+        <v>115</v>
+      </c>
+      <c r="BY61" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ61" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM61">
+        <v>0</v>
+      </c>
+      <c r="CN61">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO61" t="s">
+        <v>111</v>
+      </c>
+      <c r="CP61" t="s">
+        <v>116</v>
+      </c>
+      <c r="CQ61" t="s">
+        <v>110</v>
+      </c>
+      <c r="CR61">
+        <v>0</v>
+      </c>
+      <c r="CS61" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62">
+        <v>13</v>
+      </c>
+      <c r="BA62" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB62" t="s">
+        <v>214</v>
+      </c>
+      <c r="BC62" t="s">
+        <v>158</v>
+      </c>
+      <c r="BD62" t="s">
+        <v>158</v>
+      </c>
+      <c r="BE62" t="s">
+        <v>160</v>
+      </c>
+      <c r="BF62" t="s">
+        <v>156</v>
+      </c>
+      <c r="BG62" t="s">
+        <v>158</v>
+      </c>
+      <c r="BH62" t="s">
+        <v>161</v>
+      </c>
+      <c r="BI62" t="s">
+        <v>161</v>
+      </c>
+      <c r="BJ62" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK62" t="s">
+        <v>160</v>
+      </c>
+      <c r="BL62" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM62" t="s">
+        <v>158</v>
+      </c>
+      <c r="BY62" t="s">
+        <v>215</v>
+      </c>
+      <c r="BZ62" t="s">
+        <v>216</v>
+      </c>
+      <c r="CA62" t="s">
+        <v>126</v>
+      </c>
+      <c r="CM62">
+        <v>0.5</v>
+      </c>
+      <c r="CN62">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO62" t="s">
+        <v>165</v>
+      </c>
+      <c r="CP62" t="s">
+        <v>166</v>
+      </c>
+      <c r="CQ62" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS62" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63">
+        <v>17</v>
+      </c>
+      <c r="BY63" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ63" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB63" t="s">
+        <v>217</v>
+      </c>
+      <c r="CC63" t="s">
+        <v>218</v>
+      </c>
+      <c r="CD63" t="s">
+        <v>219</v>
+      </c>
+      <c r="CE63" t="s">
+        <v>220</v>
+      </c>
+      <c r="CF63" t="s">
+        <v>221</v>
+      </c>
+      <c r="CG63" t="s">
+        <v>222</v>
+      </c>
+      <c r="CM63">
+        <v>0</v>
+      </c>
+      <c r="CN63">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO63" t="s">
+        <v>166</v>
+      </c>
+      <c r="CP63" t="s">
+        <v>174</v>
+      </c>
+      <c r="CQ63" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS63" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64">
+        <v>18</v>
+      </c>
+      <c r="BY64" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ64" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH64" t="s">
+        <v>223</v>
+      </c>
+      <c r="CI64" t="s">
+        <v>224</v>
+      </c>
+      <c r="CJ64" t="s">
+        <v>178</v>
+      </c>
+      <c r="CK64" t="s">
+        <v>225</v>
+      </c>
+      <c r="CL64" t="s">
+        <v>226</v>
+      </c>
+      <c r="CM64">
+        <v>0</v>
+      </c>
+      <c r="CN64">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CP64" t="s">
+        <v>181</v>
+      </c>
+      <c r="CQ64" t="s">
+        <v>166</v>
+      </c>
+      <c r="CS64" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65">
+        <v>11</v>
+      </c>
+      <c r="AZ65" t="s">
+        <v>227</v>
+      </c>
+      <c r="BY65" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ65" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM65">
+        <v>0</v>
+      </c>
+      <c r="CN65">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO65" t="s">
+        <v>148</v>
+      </c>
+      <c r="CP65" t="s">
+        <v>151</v>
+      </c>
+      <c r="CQ65" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR65">
+        <v>0</v>
+      </c>
+      <c r="CS65" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="BY66" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ66" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM66">
+        <v>0</v>
+      </c>
+      <c r="CN66">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO66" t="s">
+        <v>116</v>
+      </c>
+      <c r="CP66" t="s">
+        <v>105</v>
+      </c>
+      <c r="CQ66" t="s">
+        <v>111</v>
+      </c>
+      <c r="CR66">
+        <v>0</v>
+      </c>
+      <c r="CS66" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67">
+        <v>12</v>
+      </c>
+      <c r="BY67" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ67" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM67">
+        <v>0</v>
+      </c>
+      <c r="CN67">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO67" t="s">
+        <v>151</v>
+      </c>
+      <c r="CP67" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ67" t="s">
+        <v>148</v>
+      </c>
+      <c r="CR67">
+        <v>0</v>
+      </c>
+      <c r="CS67" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>187</v>
+      </c>
+      <c r="B68" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68">
+        <v>19</v>
+      </c>
+      <c r="BY68" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ68" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM68">
+        <v>0</v>
+      </c>
+      <c r="CN68">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO68" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ68" t="s">
+        <v>151</v>
+      </c>
+      <c r="CR68">
+        <v>3</v>
+      </c>
+      <c r="CS68" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>186</v>
+      </c>
+      <c r="B69" t="s">
+        <v>228</v>
+      </c>
+      <c r="C69">
+        <v>14</v>
+      </c>
+      <c r="BY69" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ69" t="s">
+        <v>230</v>
+      </c>
+      <c r="CA69" t="s">
+        <v>201</v>
+      </c>
+      <c r="CM69">
+        <v>0.05</v>
+      </c>
+      <c r="CN69">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO69" t="s">
+        <v>231</v>
+      </c>
+      <c r="CP69" t="s">
+        <v>166</v>
+      </c>
+      <c r="CQ69" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS69" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="G70" t="s">
+        <v>102</v>
+      </c>
+      <c r="H70" t="s">
+        <v>100</v>
+      </c>
+      <c r="I70" t="s">
+        <v>102</v>
+      </c>
+      <c r="J70" t="s">
+        <v>99</v>
+      </c>
+      <c r="K70" t="s">
+        <v>101</v>
+      </c>
+      <c r="L70" t="s">
+        <v>100</v>
+      </c>
+      <c r="M70" t="s">
+        <v>103</v>
+      </c>
+      <c r="N70" t="s">
+        <v>101</v>
+      </c>
+      <c r="O70" t="s">
+        <v>100</v>
+      </c>
+      <c r="P70" t="s">
+        <v>99</v>
+      </c>
+      <c r="BY70" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ70" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM70">
+        <v>0.1</v>
+      </c>
+      <c r="CN70">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO70" t="s">
+        <v>105</v>
+      </c>
+      <c r="CP70" t="s">
+        <v>106</v>
+      </c>
+      <c r="CQ70" t="s">
+        <v>107</v>
+      </c>
+      <c r="CR70">
+        <v>0</v>
+      </c>
+      <c r="CS70" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>186</v>
+      </c>
+      <c r="B71" t="s">
+        <v>167</v>
+      </c>
+      <c r="C71">
+        <v>17</v>
+      </c>
+      <c r="BY71" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ71" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB71" t="s">
+        <v>232</v>
+      </c>
+      <c r="CC71" t="s">
+        <v>233</v>
+      </c>
+      <c r="CD71" t="s">
+        <v>234</v>
+      </c>
+      <c r="CE71" t="s">
+        <v>220</v>
+      </c>
+      <c r="CF71" t="s">
+        <v>235</v>
+      </c>
+      <c r="CG71" t="s">
+        <v>236</v>
+      </c>
+      <c r="CM71">
+        <v>0</v>
+      </c>
+      <c r="CN71">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO71" t="s">
+        <v>166</v>
+      </c>
+      <c r="CP71" t="s">
+        <v>174</v>
+      </c>
+      <c r="CQ71" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS71" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72">
+        <v>7</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>101</v>
+      </c>
+      <c r="R72" t="s">
+        <v>99</v>
+      </c>
+      <c r="S72" t="s">
+        <v>99</v>
+      </c>
+      <c r="T72" t="s">
+        <v>101</v>
+      </c>
+      <c r="U72" t="s">
+        <v>99</v>
+      </c>
+      <c r="V72" t="s">
+        <v>102</v>
+      </c>
+      <c r="W72" t="s">
+        <v>100</v>
+      </c>
+      <c r="X72" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY72" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ72" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM72">
+        <v>0.1</v>
+      </c>
+      <c r="CN72">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO72" t="s">
+        <v>106</v>
+      </c>
+      <c r="CP72" t="s">
+        <v>119</v>
+      </c>
+      <c r="CQ72" t="s">
+        <v>105</v>
+      </c>
+      <c r="CR72">
+        <v>0</v>
+      </c>
+      <c r="CS72" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>187</v>
+      </c>
+      <c r="B73" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73">
         <v>15</v>
       </c>
-      <c r="BY30" t="s">
-        <v>189</v>
-      </c>
-      <c r="BZ30" t="s">
-        <v>190</v>
-      </c>
-      <c r="CA30" t="s">
-        <v>191</v>
-      </c>
-      <c r="CM30">
-        <v>0.2</v>
-      </c>
-      <c r="CN30">
-        <v>6.1</v>
-      </c>
-      <c r="CO30" t="s">
+      <c r="BY73" t="s">
+        <v>238</v>
+      </c>
+      <c r="BZ73" t="s">
+        <v>239</v>
+      </c>
+      <c r="CA73" t="s">
+        <v>201</v>
+      </c>
+      <c r="CM73">
+        <v>0.15</v>
+      </c>
+      <c r="CN73">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO73" t="s">
+        <v>240</v>
+      </c>
+      <c r="CP73" t="s">
+        <v>166</v>
+      </c>
+      <c r="CQ73" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS73" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>209</v>
+      </c>
+      <c r="B74" t="s">
+        <v>120</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY74" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ74" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM74">
+        <v>0</v>
+      </c>
+      <c r="CN74">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO74" t="s">
+        <v>119</v>
+      </c>
+      <c r="CP74" t="s">
+        <v>123</v>
+      </c>
+      <c r="CQ74" t="s">
+        <v>106</v>
+      </c>
+      <c r="CR74">
+        <v>0</v>
+      </c>
+      <c r="CS74" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>209</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75">
+        <v>19</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE75" t="s">
+        <v>126</v>
+      </c>
+      <c r="BY75" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ75" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM75">
+        <v>0</v>
+      </c>
+      <c r="CN75">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO75" t="s">
+        <v>123</v>
+      </c>
+      <c r="CP75" t="s">
+        <v>127</v>
+      </c>
+      <c r="CQ75" t="s">
+        <v>119</v>
+      </c>
+      <c r="CR75">
+        <v>0</v>
+      </c>
+      <c r="CS75" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>186</v>
+      </c>
+      <c r="B76" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76">
+        <v>18</v>
+      </c>
+      <c r="BY76" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ76" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH76" t="s">
+        <v>242</v>
+      </c>
+      <c r="CI76" t="s">
+        <v>177</v>
+      </c>
+      <c r="CJ76" t="s">
+        <v>243</v>
+      </c>
+      <c r="CK76" t="s">
+        <v>243</v>
+      </c>
+      <c r="CL76" t="s">
+        <v>244</v>
+      </c>
+      <c r="CM76">
+        <v>0</v>
+      </c>
+      <c r="CN76">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CP76" t="s">
+        <v>181</v>
+      </c>
+      <c r="CQ76" t="s">
+        <v>166</v>
+      </c>
+      <c r="CS76" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>187</v>
+      </c>
+      <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77">
+        <v>17</v>
+      </c>
+      <c r="BY77" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ77" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB77" t="s">
+        <v>245</v>
+      </c>
+      <c r="CC77" t="s">
+        <v>246</v>
+      </c>
+      <c r="CD77" t="s">
+        <v>247</v>
+      </c>
+      <c r="CE77" t="s">
+        <v>248</v>
+      </c>
+      <c r="CF77" t="s">
+        <v>249</v>
+      </c>
+      <c r="CG77" t="s">
+        <v>250</v>
+      </c>
+      <c r="CM77">
+        <v>0</v>
+      </c>
+      <c r="CN77">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO77" t="s">
+        <v>166</v>
+      </c>
+      <c r="CP77" t="s">
+        <v>174</v>
+      </c>
+      <c r="CQ77" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS77" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>187</v>
+      </c>
+      <c r="B78" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78">
+        <v>18</v>
+      </c>
+      <c r="BY78" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ78" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH78" t="s">
+        <v>251</v>
+      </c>
+      <c r="CI78" t="s">
+        <v>252</v>
+      </c>
+      <c r="CJ78" t="s">
+        <v>253</v>
+      </c>
+      <c r="CK78" t="s">
+        <v>243</v>
+      </c>
+      <c r="CL78" t="s">
+        <v>254</v>
+      </c>
+      <c r="CM78">
+        <v>0</v>
+      </c>
+      <c r="CN78">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CP78" t="s">
+        <v>181</v>
+      </c>
+      <c r="CQ78" t="s">
+        <v>166</v>
+      </c>
+      <c r="CS78" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79">
+        <v>9</v>
+      </c>
+      <c r="AF79" t="s">
         <v>192</v>
       </c>
-      <c r="CP30" t="s">
+      <c r="AG79" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH79" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI79" t="s">
+        <v>256</v>
+      </c>
+      <c r="AJ79" t="s">
+        <v>257</v>
+      </c>
+      <c r="AK79" t="s">
+        <v>134</v>
+      </c>
+      <c r="BY79" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ79" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM79">
+        <v>0</v>
+      </c>
+      <c r="CN79">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO79" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP79" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ79" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR79">
+        <v>0</v>
+      </c>
+      <c r="CS79" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>209</v>
+      </c>
+      <c r="B80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="AP80" t="s">
+        <v>258</v>
+      </c>
+      <c r="AQ80" t="s">
+        <v>140</v>
+      </c>
+      <c r="AR80" t="s">
+        <v>259</v>
+      </c>
+      <c r="AS80" t="s">
+        <v>260</v>
+      </c>
+      <c r="AT80" t="s">
+        <v>261</v>
+      </c>
+      <c r="AU80" t="s">
+        <v>144</v>
+      </c>
+      <c r="AV80" t="s">
+        <v>145</v>
+      </c>
+      <c r="AW80" t="s">
+        <v>262</v>
+      </c>
+      <c r="BY80" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ80" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM80">
+        <v>0</v>
+      </c>
+      <c r="CN80">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO80" t="s">
+        <v>137</v>
+      </c>
+      <c r="CP80" t="s">
+        <v>148</v>
+      </c>
+      <c r="CQ80" t="s">
+        <v>127</v>
+      </c>
+      <c r="CR80">
+        <v>0</v>
+      </c>
+      <c r="CS80" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>209</v>
+      </c>
+      <c r="B81" t="s">
+        <v>149</v>
+      </c>
+      <c r="C81">
+        <v>11</v>
+      </c>
+      <c r="AZ81" t="s">
+        <v>263</v>
+      </c>
+      <c r="BY81" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ81" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM81">
+        <v>0</v>
+      </c>
+      <c r="CN81">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO81" t="s">
+        <v>148</v>
+      </c>
+      <c r="CP81" t="s">
+        <v>151</v>
+      </c>
+      <c r="CQ81" t="s">
+        <v>137</v>
+      </c>
+      <c r="CR81">
+        <v>0</v>
+      </c>
+      <c r="CS81" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82">
+        <v>12</v>
+      </c>
+      <c r="BY82" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ82" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM82">
+        <v>0</v>
+      </c>
+      <c r="CN82">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO82" t="s">
+        <v>151</v>
+      </c>
+      <c r="CP82" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ82" t="s">
+        <v>148</v>
+      </c>
+      <c r="CR82">
+        <v>0</v>
+      </c>
+      <c r="CS82" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>209</v>
+      </c>
+      <c r="B83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83">
+        <v>19</v>
+      </c>
+      <c r="BY83" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ83" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM83">
+        <v>0</v>
+      </c>
+      <c r="CN83">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO83" t="s">
+        <v>153</v>
+      </c>
+      <c r="CQ83" t="s">
+        <v>151</v>
+      </c>
+      <c r="CR83">
+        <v>4</v>
+      </c>
+      <c r="CS83" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>209</v>
+      </c>
+      <c r="B84" t="s">
+        <v>264</v>
+      </c>
+      <c r="C84">
+        <v>15</v>
+      </c>
+      <c r="BY84" t="s">
+        <v>265</v>
+      </c>
+      <c r="BZ84" t="s">
+        <v>239</v>
+      </c>
+      <c r="CA84" t="s">
+        <v>201</v>
+      </c>
+      <c r="CM84">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="CN84">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO84" t="s">
+        <v>266</v>
+      </c>
+      <c r="CP84" t="s">
         <v>166</v>
       </c>
-      <c r="CQ30" t="s">
+      <c r="CQ84" t="s">
         <v>153</v>
       </c>
-      <c r="CS30" t="b">
-        <v>1</v>
-      </c>
-      <c r="CT30">
+      <c r="CS84" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>209</v>
+      </c>
+      <c r="B85" t="s">
+        <v>167</v>
+      </c>
+      <c r="C85">
+        <v>17</v>
+      </c>
+      <c r="BY85" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ85" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB85" t="s">
+        <v>267</v>
+      </c>
+      <c r="CC85" t="s">
+        <v>268</v>
+      </c>
+      <c r="CD85" t="s">
+        <v>268</v>
+      </c>
+      <c r="CE85" t="s">
+        <v>269</v>
+      </c>
+      <c r="CF85" t="s">
+        <v>270</v>
+      </c>
+      <c r="CG85" t="s">
+        <v>235</v>
+      </c>
+      <c r="CM85">
+        <v>0</v>
+      </c>
+      <c r="CN85">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CO85" t="s">
+        <v>166</v>
+      </c>
+      <c r="CP85" t="s">
+        <v>174</v>
+      </c>
+      <c r="CQ85" t="s">
+        <v>153</v>
+      </c>
+      <c r="CS85" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:98" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>209</v>
+      </c>
+      <c r="B86" t="s">
+        <v>175</v>
+      </c>
+      <c r="C86">
+        <v>18</v>
+      </c>
+      <c r="BY86" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ86" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH86" t="s">
+        <v>271</v>
+      </c>
+      <c r="CI86" t="s">
+        <v>272</v>
+      </c>
+      <c r="CJ86" t="s">
+        <v>178</v>
+      </c>
+      <c r="CK86" t="s">
+        <v>225</v>
+      </c>
+      <c r="CL86" t="s">
+        <v>273</v>
+      </c>
+      <c r="CM86">
+        <v>0</v>
+      </c>
+      <c r="CN86">
+        <v>9.0499999999999989</v>
+      </c>
+      <c r="CP86" t="s">
+        <v>181</v>
+      </c>
+      <c r="CQ86" t="s">
+        <v>166</v>
+      </c>
+      <c r="CS86" t="b">
+        <v>1</v>
+      </c>
+      <c r="CT86">
         <v>0</v>
       </c>
     </row>

</xml_diff>